<commit_message>
Refactor RQ3 analysis folder structure and file naming conventions
</commit_message>
<xml_diff>
--- a/replication/rq3_analysis/challenges_mitigation_analysis.xlsx
+++ b/replication/rq3_analysis/challenges_mitigation_analysis.xlsx
@@ -1089,7 +1089,11 @@
           <t>Store calibrated values for stable energy consumption, maximum allowed temperatures, and wait times specific to the hardware configuration for reuse.</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>d706dc7b-10c0-4975-8b65-1b27312bb7d5</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1115,7 +1119,11 @@
           <t>Understand the expected range of variation for your hardware and incorporate that knowledge into interpreting energy measurements and making decisions.</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>4301882c-1d65-4e17-9e5a-8ec57048a83c</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">

</xml_diff>